<commit_message>
fix changer updater fix orm query for counters
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Александр\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D996CE4A-245B-4FB4-B15C-816288FB1D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,9 +31,6 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjvwozj06heQVGmxYVZutM7iYW8Dw=="/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -89,7 +86,7 @@
     <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
   </si>
   <si>
-    <t>Чиизу Рамен</t>
+    <t>Чизу Рамен</t>
   </si>
   <si>
     <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
@@ -153,18 +150,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Montserrat"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,33 +201,126 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -431,27 +529,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.574285714285713" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="77.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.428571428571429" customWidth="1"/>
+    <col min="2" max="2" width="20.857142857142858" customWidth="1"/>
+    <col min="3" max="3" width="20.142857142857142" customWidth="1"/>
+    <col min="4" max="4" width="21.714285714285715" style="3" customWidth="1"/>
+    <col min="5" max="5" width="77.71428571428571" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.571428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -465,7 +563,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="4">
         <v>1</v>
@@ -517,7 +615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -533,7 +631,7 @@
         <v>265.57</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2</v>
@@ -562,6 +660,9 @@
       <c r="F7" s="4">
         <v>166.47</v>
       </c>
+      <c r="G7">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
@@ -578,6 +679,9 @@
       <c r="F8" s="4">
         <v>168.25</v>
       </c>
+      <c r="G8">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -598,7 +702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -612,7 +716,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>1</v>
@@ -626,7 +730,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
@@ -642,7 +746,7 @@
         <v>2700.79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
@@ -677,7 +781,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>2</v>
@@ -691,7 +795,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -726,7 +830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4">
@@ -742,20 +846,20 @@
         <v>520.08000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>